<commit_message>
Created PCB Errors document
</commit_message>
<xml_diff>
--- a/411 Project/nocLock/Documentaion/System Design/Description Table.xlsx
+++ b/411 Project/nocLock/Documentaion/System Design/Description Table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12800" windowHeight="15480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="32">
   <si>
     <t>Input Name</t>
   </si>
@@ -109,6 +109,12 @@
   </si>
   <si>
     <t>nocLock</t>
+  </si>
+  <si>
+    <t>Level 0:</t>
+  </si>
+  <si>
+    <t>Level 1:</t>
   </si>
 </sst>
 </file>
@@ -161,7 +167,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -186,10 +192,77 @@
     </border>
     <border>
       <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
       <right style="medium">
         <color auto="1"/>
       </right>
       <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
         <color auto="1"/>
       </top>
       <bottom/>
@@ -203,13 +276,11 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -233,26 +304,42 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -264,6 +351,8 @@
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -275,6 +364,8 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -604,10 +695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -621,171 +712,179 @@
     <col min="7" max="7" width="32.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:6" ht="16" thickBot="1">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="31" thickBot="1">
+      <c r="A2" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D2" s="9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="45">
-      <c r="A2" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="3" t="s">
+    <row r="3" spans="1:6" ht="45">
+      <c r="A3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D3" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="60">
-      <c r="A3" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="3" t="s">
+    <row r="4" spans="1:6" ht="60">
+      <c r="A4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="60">
-      <c r="A4" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" s="3" t="s">
+    <row r="5" spans="1:6" ht="60">
+      <c r="A5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="75">
-      <c r="A5" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="105">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="75">
       <c r="A6" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="105">
+      <c r="A7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="90">
-      <c r="A7" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="3" t="s">
+    <row r="8" spans="1:6" ht="90">
+      <c r="A8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="91" thickBot="1">
-      <c r="A8" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="3" t="s">
+    <row r="9" spans="1:6" ht="91" thickBot="1">
+      <c r="A9" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C9" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D9" s="14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30">
-      <c r="A9" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="5" t="s">
+    <row r="10" spans="1:6" ht="31" thickBot="1">
+      <c r="A10" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C10" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D10" s="15" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="75">
-      <c r="A10" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="3" t="s">
+    <row r="11" spans="1:6" ht="75">
+      <c r="A11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D11" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="75">
-      <c r="A11" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="3" t="s">
+    <row r="12" spans="1:6" ht="75">
+      <c r="A12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="60">
-      <c r="A12" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="60">
+      <c r="A13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>